<commit_message>
TEC-330. Registrar usuario desde backoffice. Incluye pre-inscripto como opción de estado en inscripciones, solo cuando corresponde. Incluye visualizar datos básicos de usuario.
</commit_message>
<xml_diff>
--- a/resources/templates/importar_inscripciones_template.xlsx
+++ b/resources/templates/importar_inscripciones_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/code/atlas/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="-18000" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>punto</t>
-  </si>
-  <si>
     <t>grupo</t>
   </si>
   <si>
@@ -54,6 +51,24 @@
   </si>
   <si>
     <t>&lt;-- NO CAMBIAR TITULOS</t>
+  </si>
+  <si>
+    <t>presente</t>
+  </si>
+  <si>
+    <t>pago</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>[Si / No]</t>
+  </si>
+  <si>
+    <t>[Sin Contactar, Sin Interés, Sin Confirmar, Confirmado]</t>
+  </si>
+  <si>
+    <t>punto de encuentro</t>
   </si>
 </sst>
 </file>
@@ -394,49 +409,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="64.83203125" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>